<commit_message>
this works, just not ios save image
</commit_message>
<xml_diff>
--- a/docs/data/excel/call_book.xlsx
+++ b/docs/data/excel/call_book.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>filename</t>
   </si>
@@ -194,6 +194,351 @@
   </si>
   <si>
     <t>花蝴蝶</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M01-夜狩.png</t>
+  </si>
+  <si>
+    <t>B.Rise，16人曲，Team B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在一片荒芜中睁眼
+寻找填满饥饿的一切
+废土吞噬世界
+我只能将信念反复咀嚼
+像只野兽蛰伏在黑夜
+冰冷无慈悲的狩猎
+是生存或嗜血
+我没想过辩解
+当我抬头质问苍穹
+是否偷走我的梦
+所以才躲那么远
+不让我利爪触碰
+无数次的冲撞牢笼
+吞下所有伤痛
+命运残酷却也夺不走我眼底的星空
+直面荒诞不经的威胁
+报以弱肉强食的哲学
+求饶换来欺蔑
+这种剧情只会一再上演
+不是与生俱来的顽劣
+只是我学不会妥协
+撕咬这个世界
+直到獠牙断裂
+当我抬头质问苍穹
+是否偷走我的梦
+所以才躲那么远
+不让我利爪触碰
+无数次的冲撞牢笼
+吞下所有伤痛
+命运残酷却也夺不走我眼底的星空
+当我抬头质问苍穹
+是否偷走我的梦
+所以才躲那么远
+不让我利爪触碰
+无数次的冲撞牢笼
+吞下所有伤痛
+命运残酷却也夺不走我眼底的星空
+</t>
+  </si>
+  <si>
+    <t>夜狩</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M02-B.Rise.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">谁说火和冰配在一起 生命会被消耗殆尽
+说到底是没有人相信 碰撞会诞生最强属性
+黎明前夕所有常理都是过去
+机械记忆分崩离析重构定义
+陈旧规矩有害垃圾词不达意
+而我和你向着晨曦迎风立旗
+像流星雨夜 要旧世湮灭 碰撞一个美丽新世界
+重建这一切 冰冷而炽烈 要着条条框框全瓦解
+高墙会更迭 王冠即废铁 谁配定义完美或残缺
+挥毫破热血 由我们来写 前人所未闻的全新章节
+是出路或末路 赢或输没退路
+一边腥风血雨 一边跳舞
+冰与火 你和我 对或错 不在乎
+既要重塑 先踏上旅途
+我们存在就像可燃冰 是指向未来的奇迹
+从深海与冻土中苏醒 奏响通往明天的序曲
+黎明前夕所有常理都是过去
+机械记忆分崩离析重构定义
+陈旧规矩有害垃圾词不达意
+而我和你向着晨曦迎风立旗
+像流星雨夜 要旧世湮灭 碰撞一个美丽新世界
+重建这一切 冰冷而炽烈 要着条条框框全瓦解
+高墙会更迭 王冠即废铁 谁配定义完美或残缺
+挥毫破热血 由我们来写 前人所未闻的全新章节
+是出路或末路 赢或输没退路
+一边腥风血雨 一边跳舞
+冰与火 你和我 对或错 不在乎
+既要重塑 先踏上旅途
+像流星雨夜 要旧世湮灭 碰撞一个美丽新世界
+重建这一切 冰冷而炽烈 要着条条框框全瓦解
+高墙会更迭 王冠即废铁 谁配定义完美或残缺
+挥毫破热血 由我们来写 前人所未闻的全新章节
+是出路或末路 赢或输没退路
+一边腥风血雨 一边跳舞
+冰与火 你和我 对或错 不在乎
+既要重塑 先踏上旅途
+</t>
+  </si>
+  <si>
+    <t>B.Rise</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M03-不死鸟.png</t>
+  </si>
+  <si>
+    <t>Woooo~~~~~
+干瘪的改装轮胎
+碾过废墟的尘埃
+黄沙之外 我很期待
+前方有什么阻碍
+良知变异的时代
+混乱在优胜劣汰
+人生好坏 不能空白
+没想过活着离开
+我如野火不请自来 
+Woooo
+携狂风放一片火海
+反正旧世已破败
+不如掀桌重开
+我要眼前
+燃烧 这世界 燃烧 这一切
+要业火如浪红莲翻赤潮
+燃烧 我自己 燃烧成灰烬
+临界淬火我挥向命运的刀
+燃烧 这世界 燃烧 这一切
+分不清热浪咆哮或狂笑
+一切都烧掉
+平静了尘嚣
+仔细听这灰烬中鸣叫
+那就是我 burn it all
+重生都始于破坏
+负担太多会过载
+荒诞时代 皆是尘埃
+没人能置身事外
+我像野火不请自来
+Woooo
+携狂风撒一片火海
+反正旧世已破败
+不如掀桌重开
+我要眼前
+燃烧 这世界 燃烧 这一切
+要业火如浪红莲翻赤潮
+燃烧 我自己 燃烧成灰烬
+临界淬火我挥向命运的刀
+燃烧 这世界 燃烧 这一切
+分不清热浪咆哮或狂笑
+烧尽 我的心 烧光 我的名
+将陈旧的所有悉数烧焦
+反正旧世已破败
+不如掀桌重开
+我要眼前
+燃烧 这世界 燃烧 这一切
+要业火如浪红莲翻赤潮
+燃烧 我自己 燃烧成灰烬
+临界淬火我挥向命运的刀
+燃烧 这世界 燃烧 这一切
+分不清热浪咆哮或狂笑
+一切都烧掉
+平静了尘嚣
+仔细听这灰烬中鸣叫
+那就是我 burn it all
+Woooo~~~~~</t>
+  </si>
+  <si>
+    <t>不死鸟</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M04-荒火.png</t>
+  </si>
+  <si>
+    <t>谁让虚伪还没腐蚀我的脊椎
+Woo
+谁让卑躬屈膝谄媚我学不会
+Woo
+Let us play the game
+我的逻辑非常简单
+所谓世界观主打向前不拐弯
+别管鲁莽还是勇敢
+不先碎成灰
+又从哪里涅槃
+Hey
+解剖开我的血管
+勇气和碳酸
+占了四分之三
+Hey
+与其苟延残喘
+不如适当野蛮
+让我神聚形散
+野火就是会这样死灰复燃
+谁让虚伪还没腐蚀我的脊椎
+Woo（无所畏）
+谁让卑躬屈膝谄媚我学不会
+Woo（不后退）
+叫我无名之辈
+等我慢慢烧毁
+虚构的高贵
+等你发现包围早已无路可退
+Let us burn the game
+就像不可控的变换
+但放大了看只不过是某种循环
+想理解我并不困难
+是为了重生
+而毁灭的必然
+Hey
+解剖开我的血管
+勇气和碳酸
+占了四分之三
+Hey
+与其苟延残喘
+不如适当野蛮
+让我神聚形散
+野火就是会这样死灰复燃
+谁让虚伪还没腐蚀我的脊椎
+Woo（无所畏）
+谁让卑躬屈膝谄媚我学不会
+Woo（不后退）
+叫我无名之辈
+等我慢慢烧毁
+虚构的高贵
+等你发现包围早已无路可退
+Let us burn the game
+谁让虚伪还没腐蚀我的脊椎
+Woo（无所畏）
+谁让卑躬屈膝谄媚我学不会
+Woo（不后退）
+叫我无名之辈
+等我慢慢烧毁
+虚构的高贵
+等你发现包围早已无路可退
+Let us burn the game</t>
+  </si>
+  <si>
+    <t>荒火</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M05-自我定义.png</t>
+  </si>
+  <si>
+    <t>B.Rise，Unit，Team B</t>
+  </si>
+  <si>
+    <t>窃窃私语just to diss 微妙的空气
+装成顺应的贬义 充斥着算计
+看破懒得说破 回避不等于懦弱
+我不屑戳穿暗地揶揄的龌龊
+难以融入规则 突兀的角色
+但所谓的不契合 标准是如何
+被视为怪异的存在
+没错确实我是这种存在
+无法被捏造的存在
+再违和也 要存在
+Through my eyes
+Hey 我会定夺过错与对
+Hey 无端指责 别来招惹
+Never never
+我会自己主导
+Beat it down Beat it down
+Beat it down Beat it down
+我有我之道 不用谁指导
+Shut up Shut up
+评头论足的丑态
+就像正在 求注目的乞丐
+You can try
+不用光躲在背后 Let it show
+想上蹿下跳就表演个够
+刺耳干扰分贝 我没空理会
+I've got something to say 只是你不配
+谁想左右我的节奏
+抱歉现在是完全失控节奏
+桀骜不驯我的节奏
+我行我素 这节奏
+Hit the road
+Hey 我会定夺过错与对
+Hey 无端指责 别来招惹
+Never never
+我会自己主导
+Beat it down Beat it down
+Beat it down Beat it down
+我有我之道 不用谁指导
+Shut up Shut up
+径直走 不回头
+Wu 不想改 不会改
+永远都 不回头
+Wu Forever goodbye
+Hey 我会定夺过错与对
+Hey 无端指责 别来招惹
+Never never
+我会自己主导
+Beat it down Beat it down
+Beat it down Beat it down
+我有我之道 不用谁指导
+Shut up Shut up
+Shut up</t>
+  </si>
+  <si>
+    <t>自我定义</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M06-偶像宣言.png</t>
+  </si>
+  <si>
+    <t>在可爱被淘汰 卖萌无效的时代
+难道还有人会期待 纯情告白
+更迭得太快 确实会无奈
+可我仍想呐喊 就现在
+被模糊的定义 会再次清晰
+幻想的勇气 泪的魔力
+一直坚持 不合时宜
+即使过了期限 梦也未曾改变
+Oh yeah oh yeah Never die
+用最纯粹的笑颜瞬间就能让回忆浮现
+趁着光芒还在 任性地盛开
+真心别掩盖 请用力喝彩
+与其叹息怀念 不如重新超越
+Oh yeah oh yeah Overdrive
+用最响亮的分贝要大声说出好久都不见
+无论哪个时代 都抹不去的色彩
+热忱不败
+Oh yeah oh yeah One more try
+当风抚平裙摆 吹散了刘海
+（Yes）其实我全都明白
+（No）但初心无可替代
+就算偏执换取不到偏爱
+我也依然果断 就现在
+被遗忘的心意 会再次响起
+无限的元气 梦的距离
+成为偶像的不可思议
+从来不被磨灭 这份憧憬雀跃
+Oh yeah oh yeah Overfly
+用最诚挚的诺言跟你约好了总有一天
+会在每个时代 永远闪耀的存在
+梦想不败
+Oh yeah oh yeah On my side
+像从前不害怕
+向着天空出发
+Go！Go！Lalalala
+再一次奔跑吧
+即使过了期限 梦也未曾改变
+yeah yeah Never die
+用最纯粹的笑颜瞬间就能让回忆浮现
+趁着光芒还在 任性地盛开
+真心别掩盖 请用力喝彩
+与其叹息怀念 不如重新超越
+Oh yeah oh yeah Overdrive
+用最响亮的分贝要大声说出好久都不见
+无论哪个时代 都抹不去的色彩
+热忱不败
+Oh yeah oh yeah One more try</t>
+  </si>
+  <si>
+    <t>偶像宣言</t>
   </si>
 </sst>
 </file>
@@ -1202,17 +1547,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" customHeight="1" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="15.9196428571429" customWidth="1"/>
+    <col min="1" max="1" width="32.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="28.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="36.5982142857143" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="18.75" customWidth="1"/>
     <col min="5" max="5" width="24.2589285714286" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1259,6 +1605,93 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" customHeight="1" spans="3:3">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:4">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:4">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:4">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:4">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
better search (hope so)
</commit_message>
<xml_diff>
--- a/docs/data/excel/call_book.xlsx
+++ b/docs/data/excel/call_book.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>filename</t>
   </si>
@@ -539,6 +539,634 @@
   </si>
   <si>
     <t>偶像宣言</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M07.Far away（遥不可及）.png</t>
+  </si>
+  <si>
+    <t>手 在玻璃雾气上画心
+窗外春雨淅沥低语
+情愫很莫名
+我看向你
+每次相遇
+对视让我 忐忑不已 害怕被你发现
+又期待被回应
+言语 却总在擦肩瞬间失灵
+或许只有收货心碎
+才懂距离可贵
+尝试幻想每种结尾
+再卑微的自我陶醉
+Far away
+I'm on my way
+追逐凄美的误会
+直到玫瑰全都枯萎
+就不会显得狼狈
+Far away
+I'm on my way
+藏住的真心 应该不算浪费
+Far away Away Away
+你 像是藏在咖啡杯底
+没有被搅开的糖粒
+是种只属于
+我的惊喜
+想要靠近却又担心
+破坏了这距离
+会不会眼前的诗意就会分崩离析
+Far away
+I'm on my way
+追逐凄美的误会
+直到玫瑰全都枯萎
+就不会显得狼狈
+Far away
+I'm on my way
+藏住的真心 应该不算浪费
+Far away Away Away
+如果只把你 留在回忆
+就不会叹息
+像泡沫不破才美丽
+Far away
+I'm on my way
+追逐凄美的误会
+直到玫瑰全都枯萎
+就不会显得狼狈
+Far away
+I'm on my way
+藏住的真心 应该不算浪费
+Far away Away Away
+Far away
+I'm on my way
+追逐凄美的误会
+直到玫瑰全都枯萎
+就不会显得狼狈
+Far away
+I'm on my way
+藏住的真心 应该不算浪费
+Far away Away Away</t>
+  </si>
+  <si>
+    <t>Far Away</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M08.Pick Up The PHONE.png</t>
+  </si>
+  <si>
+    <t>L-O-V-E
+Hey girl
+莫非连简单问候
+也要反复练习才开口
+Do not Do not
+不能让机会溜走
+天时地利紧要的关头
+I know I know
+Ring ring ring ring
+瞬间周围世界无比安静
+Ring ring ring ring
+心疯狂预警
+双眼紧闭屏住呼吸
+献上全部勇气
+Tell me baby
+准备好坚定的郑重回答
+Pick up pick up pick up
+这次别再装傻
+不需要谨慎地试探想法
+Pick it pick it pick it up
+Pick it pick it pick up the love
+Pick up pick up pick up the phone
+Pick up pick up pick up pick up the love
+Pick up pick up pick up the phone
+Pick up pick up pick up pick up the love
+Hey girl
+等待接通的每一刻
+都期待着
+调整到最温柔音色
+氛围吻合
+或许有默契感应
+或许吸引力早已经共鸣
+可是心意
+果然还是想直接传递oh
+恋爱宣言该被认真聆听
+Ring ring ring ring
+我决心已定
+告诉自己大胆出击
+幻想拥有魔力
+Tell me baby
+准备好坚定的郑重回答
+Pick up pick up pick up
+这次别再装傻
+不需要谨慎地试探想法
+Pick it pick it pick it up
+Pick it pick it pick up the love
+正在接通 遐想跃动
+此刻也许你也相同
+最佳坦白机会 不会错过绝对
+利落干脆
+心跳已做好准备 now
+准备好坚定的郑重回答
+Pick up pick up pick up
+这次别再装傻
+不需要谨慎地试探想法
+Pick it pick it pick it up
+Pick it pick it pick up the love
+Pick up pick up pick up the phone
+Pick up pick up pick up pick up the love
+Pick up pick up pick up the phone
+Pick up pick up pick up pick up the love</t>
+  </si>
+  <si>
+    <t>Pick Up The PHONE</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M09-Got me mad（失控法则）.png</t>
+  </si>
+  <si>
+    <t>此刻 微醺的 危险的 为何燥热
+在这 微妙的 伪装的 未央旖旎夜色
+暧昧气氛袭来 错乱心跳节拍
+快一点甩开 多余的拘谨神态 Babe
+趁现在深呼吸 沉陷在朦胧里
+直白说你目的 怎么做都可以
+That'll be crazy 试探语气泄露蛛丝马迹
+Ont to the two
+逐渐拉开帷幕
+预设好的每一步
+恰好的温度
+l want you know
+眼神交错的时候
+这一瞬间已被占有 Baby
+（Baby）
+One to the two
+逐渐混入迷雾
+预设好了下一步
+模糊了尺度
+I want to know
+指尖触碰的时候
+什么都无需理由 Baby
+I want you to
+Got me got me got me mad
+Got me got me got me mad
+Got me got me got me mad mad
+Uh Got me got me got me mad
+Got me got me got me mad
+Got me got me got me mad mad
+All l wan All l need
+What's you waiting for
+Anyone Anytime
+What you wanna meet
+花瓣凌乱散开 底线已然摊牌
+会屏息等待 狂欢的时刻到来 Babe
+遇见你已动心 预见你也倾心
+臣服式的着迷 不反抗的进击
+一缕优雅轻柔 却能惊醒沉睡野兽 oh
+One to the two
+逐渐拉开帷幕
+预设好的每一步
+恰好的温度
+l want you know
+眼神交错的时候
+这一瞬间已被占有 Baby
+I want you to
+Got me got me got me mad
+Got me got me got me mad
+Got me got me got me mad mad
+Uh
+Got me got me got me mad
+Got me got me got me mad
+Got me got me got me mad mad
+Uh oh
+被点燃的爱
+眩目虚幻的色彩
+多嚣张绮丽 burn for me burn for me
+映入了眼眸
+将所有 无法得到的渴求
+和所有 早该舍弃的残留
+Burn it if you can
+Show me if you can
+Gonna crazy with me with me
+Wanna go high
+One to the two
+逐渐混入迷雾
+预设好了下一步
+模糊了尺度
+I want to know
+指尖触碰的时候
+什么都无需理由 Baby
+I want you to
+Got me got me got me mad
+Got me got me got me mad
+Got me got me got me mad mad
+Uh Got me got me got me mad
+Got me got me got me mad
+Got me got me got me mad mad</t>
+  </si>
+  <si>
+    <t>Got me mad</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M10-草莓味的颜色.png</t>
+  </si>
+  <si>
+    <t>喜欢后的空格 是草莓成熟的颜色
+喜欢后的空格 是每次与你不谋而合
+这份憧憬心意的表达
+用哪种修辞手法
+想装作不经意 语气却很刻意
+也许还是缺少勇气 对不起
+气氛并非预想中的尴尬
+准备的台词却只剩乱码
+忽然结巴 简单逻辑也变得好复杂
+背对背 快调整呼吸
+怎么办 不然先藏好焦急
+但我回头看见 你微笑的瞬间
+犹豫的 执拗的 纠结 不安的心
+全都清零
+喜欢后的空格
+是每次与你不谋而合 wow wow wow
+我终于鼓起勇气抬头看
+你坚定的视线也绝不是偶然
+喜欢后的空格
+是温柔的无可奈何 wow wow wow
+任性的 鲜明的 别扭的 可爱的
+我要把无限空白写满
+形容你的答案
+这一次你不用太快回答
+否则矜持都没办法
+好像你没注意 或者也是有意
+将我所有慌张包庇 没关系
+煎熬就是对迟疑的惩罚
+所以我不想拖延一刹那
+因为会怕 直觉有万分之一的误差
+背对背 快调整呼吸
+怎么办 不然先藏好焦急
+但我回头看见 你微笑的瞬间
+在意的 执着的 想念的 无比期待的
+全都来自你
+喜欢后的空格
+是草莓成熟后的颜色 wow wow wow
+或许时机尚早恋爱也未满
+但心动已将甜蜜的红晕渲染
+喜欢后的空格
+是每首你哼过的歌 wow wow wow
+悸动的 轻快的 青涩的 唯美的
+我想用关于你的灵感
+描绘梦中的浪漫
+某一天忽然间 想尝试勇敢做哪怕一点改变
+思考我们之间 无数可能性的未来每天
+不止单纯的喜欢你（每一面的你）
+不设范围的主观题（每一天的你）
+一直会故意留白那憧憬心意 ahh
+喜欢后的空格
+是草莓成熟后的颜色
+或许时机尚早恋爱也未满
+但心动已将甜蜜的红晕渲染
+喜欢后的空格
+你希望我写什么呢
+真挚的 肤浅的 夸张的 会心一笑的
+万千含义 不止于你
+喜欢后的空格
+是每次与你不谋而合 wow wow wow
+我终于鼓起勇气抬头看
+你坚定的视线也绝不是偶然
+喜欢后的空格
+是温柔的无可奈何 wow wow wow
+任性的 鲜明的 别扭的 可爱的
+我要把无限空白写满
+形容你的答案
+关于你的答案
+属于我们的答案
+喜欢后的名词 一直都会有你的名字</t>
+  </si>
+  <si>
+    <t>草莓味的颜色</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M11-Final 奔向落日.png</t>
+  </si>
+  <si>
+    <t>地平线被暖色晕染
+转眼将逝的绚烂
+尽全力奔跑向海岸
+倔强依然
+想放弃其实很简单
+但还是会有期盼
+所以我
+继续向前哪怕每次都为时已晚
+机会运气时间总是不太够
+追逐的幻想会忽然变海市蜃楼
+可是我也不能再回头
+落日被海面吞没陷入黑暗之前
+我会再一次来到你的身边
+l'll be l'll be l'll be l'll be
+约定好的这天
+既然说过了再见那就一定会再见
+不顾一切去证明迟来的是诺言
+奔向你 奔向你
+一起奔赴的终点
+曾经我对天空歌唱
+多少落寞与迷茫
+好像只有去到远方
+梦才滚烫
+我想要像以前那样
+一直站在你身旁
+让夕阳
+照亮那尘封的吉他和梦想
+忘掉所有只管继续奔走
+无限拉长的影子直到城市尽头
+没有再停下的理由
+落日被海面吞没陷入黑暗之前
+我会再一次来到你的身边
+l'll be l'll be l'll be l'll be
+约定好的这天
+既然说过了再见那就一定会再见
+不顾一切去证明迟来的是诺言
+奔向你 奔向你
+一起奔赴的终点
+耳边拂过的风也为我伴奏
+这次我会毫不犹豫坚定说出口
+一定会奔向你最后
+落日被海面吞没于交替瞬间
+会如约而至出现在你眼前
+l'll be l'll be l'll be l'll be
+终点亦是原点
+因为说好了再见那就一定要再见
+执着的信念并不是谎言
+想见你 想见你
+想和你 想和你
+一起奔向明天</t>
+  </si>
+  <si>
+    <t>奔向落日</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M12-星光环绕的孤岛.png</t>
+  </si>
+  <si>
+    <t>像曾经做过的梦那样
+一瞬间被点亮了幻想
+伫立在舞台中央
+被星光一直环绕的地方
+无论将来会是怎样
+黯淡或者更加闪亮
+此刻我要大声尽情歌唱
+被黑暗局限的视野
+却有微光从未熄灭
+直到某刻当我察觉
+并非处于孤单结界
+寂寞失落的边缘
+依然紧握渺小心愿
+想要被看见的执念
+从未改变
+在晚风轻拂的夏夜
+第一次任性脱掉了凉鞋
+浪花未能将心冷却
+依旧还在崩腾不绝
+一个人对着海面
+忘我沉浸起舞翩翩
+妄想会有某天
+让梦悄然实现
+要经历多少忽视沉默
+等待才会有结果
+或许不应该思虑太多
+偶然间就会遇见流星划过
+当看见远处浮现光芒 辉映着不停歇的波浪
+会将憧憬和希望 变幻成此刻泪花的形状
+呐喊声在耳边回荡 仿佛坚持终有反响
+我也拥有了腾跃的能量
+像曾经做过的梦那样 一瞬间被点亮了幻想
+伫立在舞台中央 被星光一直环绕的地方
+无论将来会是怎样 黯淡或者更加闪亮
+此刻我要大声尽情歌唱
+在晚风轻拂的夏夜
+第一次任性脱掉了凉鞋
+浪花未能将心冷却
+依旧还在崩腾不绝
+一个人对着海面
+忘我沉浸起舞翩翩
+妄想会有某天
+让梦悄然实现
+要经历多少忽视沉默
+等待才会有结果
+或许不应该思虑太多
+偶然间就会遇见流星划过
+当看见远处浮现光芒 辉映着不停歇的波浪
+会将憧憬和希望 变幻成此刻泪花的形状
+呐喊声在耳边回荡 仿佛坚持终有反响
+我也拥有了腾跃的能量
+像曾经做过的梦那样 一瞬间被点亮了幻想
+伫立在舞台中央 被星光一直环绕的地方
+无论将来会是怎样 黯淡或者更加闪亮
+此刻我要大声尽情歌唱</t>
+  </si>
+  <si>
+    <t>星光环绕的孤岛</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M13-BETTER THAN BEST.png</t>
+  </si>
+  <si>
+    <t>当我茫然自己是为何而来的时候
+就会回想坚持这每一步的理由
+或许已经不会再有退路在我身后
+所以即使要抓住荆棘也不会放手
+对于梦想应该怎样去理解
+更高处看到的天空是否会有区别
+即便等我抵达传说中的那个世界
+已经找不到那欣欣向荣的一切
+心再渺小的力量也不枯竭
+哪怕在无尽长夜
+面临荒芜但幸好前路并未断绝
+任汗水模糊了视线方向也不会改变
+以我全部换一次孤注尝试去超越
+越过曾经被认定是最高处的山巅
+所有的人都说故事已完结
+该付出多少代价才能把历史续写
+而如今我好像也已经不在意痛觉
+以希望的名义依旧奔腾着热血
+心再渺小的力量也不枯竭
+哪怕在无尽长夜
+我会去到更高处看一看那片天
+比谁都抢先一步攀登眺望向更远
+就算留给我的仅剩转瞬的时间
+也要在最后一刻之前让梦得以成全
+顶峰停留不应该是我追求的终点
+而是要再一次破茧去飞跃的起点
+当我终于笃定自己为何而来的时候
+无需多余理由尽管继续远走
+当我决心不会留遗憾也不会再回头
+好像所谓梦想其实我早已拥有</t>
+  </si>
+  <si>
+    <t>Better Than Best</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M14-门.png</t>
+  </si>
+  <si>
+    <t>我 沐浴冰凉的雨点
+破开土睁开眼
+只为了 和传说中的人并肩
+她 却好像听不见
+与我渐行渐远
+重重关上我心里那扇门
+门那边的人 是传说
+门那边的人 让我失落
+门那边的人 总沉默
+可我听说
+门那边 有梦野千里
+它真的属于我吗
+躲在前人荣光里
+让我日渐失去勇气
+谁能够开启
+为何他们说我不配呢
+难道我还不够笨
+不够炙热
+我 寻找雷霆和闪电
+经过冰与火淬炼
+找到了 同样失落的你并肩
+我 不再怕被灼伤
+因为那一束光
+不见得 比你的眼更闪亮
+门这边的人 感动我
+门这边的人 懂我失落
+门这边的人 不沉默
+让我相信
+门那边 有梦野千里
+它真的属于我吗
+门的这边却有你
+让我获得新的勇气
+谁能够开启
+现在还有什么重要呢
+我们早就一样笨
+一样炙热
+从来就没有 一扇门
+只有能不能 触及灵魂
+当我去跨过 某扇门
+不如宣称
+我脚下 是梦野千里
+它真的属于我们
+继续唱哭一座城
+瓦解所有桎梏的门
+让我们开启
+新的纪元现在就启程
+我们还是那样笨
+笨到沸腾</t>
+  </si>
+  <si>
+    <t>门</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M15.人海一粟.png</t>
+  </si>
+  <si>
+    <t>梦深处 是我渴望的全部 或是片荒芜
+身后每一步 消融在无边迷雾
+心跳的频度 仿佛依旧不甘愿被现实说服
+再向前一步 以终章为序幕
+不知不觉被淹没在汹涌的人潮里
+连前路视线也都变得不清晰
+尝试着拼尽全力 不顾一切拨开拥挤
+总有天要从这无望的轮回逃离
+在漠然的世界里
+逐渐失去了锐利 毫不起眼的自己
+像无声叹息 汪洋中的水滴
+可是我仍想证明存在的意义
+我不怕 即便前方是断壁悬崖
+再挣扎 也不停下逞强的步伐
+泪水啊 比起虚度蒸发我更想在征途中挥洒
+选择哪一种活法 请听我的回答 
+Ha Ah～
+时间似乎被封印在熙攘的人潮里
+被束缚在这了无生机的原地
+尝试着拼尽全力 哪怕黑暗没有缝隙
+也相信能等到偶然的万分之一
+在凝固的世界里
+麻木同化的定义 随时都会被代替
+想自由呼吸 反向的目的地
+才是我作为自己存在的意义
+我不怕 即便前方是断壁悬崖
+再挣扎 也不停下逞强的步伐
+泪水啊 比起虚度蒸发我更想在征途中挥洒
+选择哪一种活法 请听我的回答
+穿越人海我我不再害怕
+未知远方有梦归处等候我抵达
+不后悔每一次出发
+是我的回答
+冲出人海如愿一刹那
+会看见梦无限大
+曾经自我激励那些话
+也早已给出了回答
+我不怕 即便前方是断壁悬崖
+再挣扎 也不停下逞强的步伐
+泪水啊 比起虚度蒸发我更想在征途中挥洒
+选择哪一种活法 请听我的回答
+给自己的回答</t>
+  </si>
+  <si>
+    <t>人海一粟</t>
+  </si>
+  <si>
+    <t>B.Rise call本_M16.弧线.png</t>
+  </si>
+  <si>
+    <t>Wow
+Wow
+我曾在泥潭中垂钓星空
+你也曾在深渊里打捞彩虹
+其实原来我们没有 彼此想象中那么不同
+都在追逐自己的梦
+黄粱一梦 也要勇 敢向前冲
+不辜负心脏的跳动
+我们会奔向不同的终点
+抬头也在看同一片蓝天
+不管时间 给什么历练
+曾许下 的誓言 我们不会变
+会有一天挣脱重力的茧
+绘画出星群迁徙的弧线
+像蒲公英 乘着风冒险
+我们会 飞很远 比永远还远
+Wow
+Wow
+Dadada～
+Dadada～
+就算要睁开眼在黑暗之中
+也一定会有光点镌刻进眼眸(你在我的眼眸)
+未来当然磕磕碰碰 正因我们会一 起度过
+所以才更值得感动
+黄粱一梦 也要勇 敢向前冲
+不辜负心脏的跳动
+我们会奔向不同的终点
+抬头也在看同一片蓝天
+不管时间 给什么历练
+曾许下 的誓言 我们不会变
+会有一天挣脱重力的茧
+绘画出星群迁徙的弧线
+像蒲公英 乘着风冒险
+我们会 飞很远 比永远还远
+Wow
+Wow
+Wow
+（还有新的冒险）
+Wow
+Wow
+Wow
+我们会奔向不同的终点
+抬头也在看同一片蓝天
+不管时间 给什么历练
+曾许下 的誓言 我们不会变
+会有一天挣脱重力的茧
+绘画出星群迁徙的弧线
+像蒲公英 乘着风冒险
+我们会 飞很远 比永远还远
+Wow
+Wow
+Dadada～
+Dadada～
+Wow
+Wow
+Dadada～
+Dadada～</t>
+  </si>
+  <si>
+    <t>弧线</t>
   </si>
 </sst>
 </file>
@@ -1547,15 +2175,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="32.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="47.6160714285714" customWidth="1"/>
     <col min="2" max="2" width="28.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="36.5982142857143" customWidth="1"/>
     <col min="4" max="4" width="18.75" customWidth="1"/>
@@ -1692,6 +2320,146 @@
         <v>31</v>
       </c>
     </row>
+    <row r="11" customHeight="1" spans="1:4">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:4">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:4">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:4">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:4">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:4">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:4">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:4">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:4">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:4">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>